<commit_message>
pre-seleccion de variables y reconstruccion de variables
</commit_message>
<xml_diff>
--- a/Diccionario-variables.xlsx
+++ b/Diccionario-variables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Esteban\Documents\Pruebas-Tecnicas\Davivienda\Esp-Analitica\forecast-home-prices\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{623474FA-349E-497E-97AE-840CB791372D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEC097B6-A621-46DF-8439-FCD8F76DF518}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{F9754126-5457-4427-B872-648245206441}"/>
   </bookViews>
@@ -761,7 +761,7 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
@@ -1098,9 +1098,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A506CE7-55E1-41AA-9512-D110FA667D4D}">
-  <dimension ref="A1:B154"/>
+  <dimension ref="A1:B161"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="A51" sqref="A51"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1542,7 +1544,7 @@
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B55" s="1" t="s">
         <v>123</v>
@@ -1550,7 +1552,7 @@
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B56" s="1" t="s">
         <v>124</v>
@@ -1558,7 +1560,7 @@
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="B57" s="2" t="s">
         <v>125</v>
@@ -1566,7 +1568,7 @@
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="B58" s="1" t="s">
         <v>126</v>
@@ -1574,7 +1576,7 @@
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="B59" s="1" t="s">
         <v>127</v>
@@ -1582,7 +1584,7 @@
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="B60" s="1" t="s">
         <v>128</v>
@@ -1590,7 +1592,7 @@
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
-        <v>60</v>
+        <v>67</v>
       </c>
       <c r="B61" s="1" t="s">
         <v>129</v>
@@ -1598,7 +1600,7 @@
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="B62" s="1" t="s">
         <v>130</v>
@@ -1606,114 +1608,93 @@
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
-        <v>62</v>
+        <v>69</v>
       </c>
       <c r="B63" s="1" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A64" s="2" t="s">
-        <v>63</v>
-      </c>
       <c r="B64" s="1" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A65" s="2" t="s">
-        <v>64</v>
-      </c>
+    <row r="65" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B65" s="1" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A66" s="2" t="s">
-        <v>65</v>
-      </c>
+    <row r="66" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B66" s="1" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A67" s="2" t="s">
-        <v>66</v>
-      </c>
+    <row r="67" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B67" s="1" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A68" s="2" t="s">
-        <v>67</v>
-      </c>
+    <row r="68" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B68" s="1" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A69" s="2" t="s">
-        <v>68</v>
-      </c>
+    <row r="69" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B69" s="1" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A70" s="2" t="s">
-        <v>69</v>
-      </c>
+    <row r="70" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B70" s="1" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B71" s="1" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B72" s="1" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B73" s="1" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B74" s="1" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B75" s="1" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B76" s="1" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="77" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B77" s="1" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="78" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B78" s="1" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="79" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B79" s="1" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="80" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B80" s="1" t="s">
         <v>148</v>
       </c>
@@ -2086,6 +2067,41 @@
     <row r="154" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B154" s="1" t="s">
         <v>222</v>
+      </c>
+    </row>
+    <row r="155" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B155" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="156" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B156" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="157" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B157" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="158" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B158" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="159" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B159" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="160" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B160" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="161" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B161" s="2" t="s">
+        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
estandarización y categorizacion de variables
</commit_message>
<xml_diff>
--- a/Diccionario-variables.xlsx
+++ b/Diccionario-variables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Esteban\Documents\Pruebas-Tecnicas\Davivienda\Esp-Analitica\forecast-home-prices\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEC097B6-A621-46DF-8439-FCD8F76DF518}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C91863B9-FD31-4E2C-909B-65D965990135}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{F9754126-5457-4427-B872-648245206441}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="256">
   <si>
     <t>variables_incluye</t>
   </si>
@@ -705,6 +705,105 @@
   </si>
   <si>
     <t>valor_avaluo_en_uvr</t>
+  </si>
+  <si>
+    <t>departamentos</t>
+  </si>
+  <si>
+    <t>VALLE DEL CAUCA</t>
+  </si>
+  <si>
+    <t>QUINDIO</t>
+  </si>
+  <si>
+    <t>ANTIOQUIA</t>
+  </si>
+  <si>
+    <t>CUNDINAMARCA</t>
+  </si>
+  <si>
+    <t>META</t>
+  </si>
+  <si>
+    <t>BOGOTA, D. C.</t>
+  </si>
+  <si>
+    <t>SANTANDER</t>
+  </si>
+  <si>
+    <t>CORDOBA</t>
+  </si>
+  <si>
+    <t>NARINO</t>
+  </si>
+  <si>
+    <t>GUAVIARE</t>
+  </si>
+  <si>
+    <t>CALDAS</t>
+  </si>
+  <si>
+    <t>BOLIVAR</t>
+  </si>
+  <si>
+    <t>ATLANTICO</t>
+  </si>
+  <si>
+    <t>TOLIMA</t>
+  </si>
+  <si>
+    <t>RISARALDA</t>
+  </si>
+  <si>
+    <t>CESAR</t>
+  </si>
+  <si>
+    <t>CASANARE</t>
+  </si>
+  <si>
+    <t>MAGDALENA</t>
+  </si>
+  <si>
+    <t>NORTE DE SANTANDER</t>
+  </si>
+  <si>
+    <t>HUILA</t>
+  </si>
+  <si>
+    <t>PUTUMAYO</t>
+  </si>
+  <si>
+    <t>CAUCA</t>
+  </si>
+  <si>
+    <t>BOYACA</t>
+  </si>
+  <si>
+    <t>SUCRE</t>
+  </si>
+  <si>
+    <t>LA GUAJIRA</t>
+  </si>
+  <si>
+    <t>AMAZONAS</t>
+  </si>
+  <si>
+    <t>CAQUETA</t>
+  </si>
+  <si>
+    <t>GUAINIA</t>
+  </si>
+  <si>
+    <t>ARAUCA</t>
+  </si>
+  <si>
+    <t>ARCHIPIELAGO DE SAN ANDRES, PROVIDENCIA Y</t>
+  </si>
+  <si>
+    <t>VICHADA</t>
+  </si>
+  <si>
+    <t>CHOCO</t>
   </si>
 </sst>
 </file>
@@ -1098,10 +1197,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A506CE7-55E1-41AA-9512-D110FA667D4D}">
-  <dimension ref="A1:B161"/>
+  <dimension ref="A1:C168"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="A51" sqref="A51"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6:A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1110,385 +1209,484 @@
     <col min="2" max="2" width="36.28515625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>78</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C9" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C12" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C13" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C14" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C15" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C16" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C17" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C18" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C19" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C20" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C21" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C22" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C23" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C24" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C25" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C26" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C27" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C28" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C29" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C30" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C31" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C32" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C33" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="B45" s="1" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="B46" s="1" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="B47" s="1" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="B48" s="1" t="s">
         <v>116</v>
@@ -1496,7 +1694,7 @@
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
-        <v>48</v>
+        <v>57</v>
       </c>
       <c r="B49" s="1" t="s">
         <v>117</v>
@@ -1504,7 +1702,7 @@
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
-        <v>49</v>
+        <v>59</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>118</v>
@@ -1512,7 +1710,7 @@
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
-        <v>50</v>
+        <v>61</v>
       </c>
       <c r="B51" s="1" t="s">
         <v>119</v>
@@ -1520,7 +1718,7 @@
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
-        <v>51</v>
+        <v>63</v>
       </c>
       <c r="B52" s="1" t="s">
         <v>120</v>
@@ -1528,7 +1726,7 @@
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
-        <v>52</v>
+        <v>65</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>121</v>
@@ -1536,7 +1734,7 @@
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
-        <v>53</v>
+        <v>67</v>
       </c>
       <c r="B54" s="1" t="s">
         <v>122</v>
@@ -1544,7 +1742,7 @@
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
-        <v>55</v>
+        <v>68</v>
       </c>
       <c r="B55" s="1" t="s">
         <v>123</v>
@@ -1552,64 +1750,43 @@
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
-        <v>57</v>
+        <v>69</v>
       </c>
       <c r="B56" s="1" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A57" s="2" t="s">
-        <v>59</v>
-      </c>
       <c r="B57" s="2" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A58" s="2" t="s">
-        <v>61</v>
-      </c>
       <c r="B58" s="1" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A59" s="2" t="s">
-        <v>63</v>
-      </c>
       <c r="B59" s="1" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A60" s="2" t="s">
-        <v>65</v>
-      </c>
       <c r="B60" s="1" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A61" s="2" t="s">
-        <v>67</v>
-      </c>
       <c r="B61" s="1" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A62" s="2" t="s">
-        <v>68</v>
-      </c>
       <c r="B62" s="1" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A63" s="2" t="s">
-        <v>69</v>
-      </c>
       <c r="B63" s="1" t="s">
         <v>131</v>
       </c>
@@ -2102,6 +2279,41 @@
     <row r="161" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B161" s="2" t="s">
         <v>64</v>
+      </c>
+    </row>
+    <row r="162" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B162" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="163" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B163" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="164" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B164" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="165" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B165" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="166" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B166" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="167" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B167" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="168" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B168" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>